<commit_message>
Fixed Jorgenson, had FeOr in the CPx test term. Now has normalized and unnormalized models.
</commit_message>
<xml_diff>
--- a/Benchmarking/clinopyroxene/Final_Versions/Jorgenson_Test_dataset.xlsx
+++ b/Benchmarking/clinopyroxene/Final_Versions/Jorgenson_Test_dataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\penny\OneDrive - Oregon State University\Postdoc\PyMME\MyBarometers\Thermobar_outer\Benchmarking\clinopyroxene\Final_Versions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52B636AE-5E43-4B87-A893-84220106B1C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91E54B38-2D88-42C1-9AE5-8628088BAB2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13290" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -147,10 +147,10 @@
     <t>FeO_Liq</t>
   </si>
   <si>
-    <t>FeOr_Cpx</t>
+    <t>Sum</t>
   </si>
   <si>
-    <t>Sum</t>
+    <t>FeOt_Cpx</t>
   </si>
 </sst>
 </file>
@@ -18330,8 +18330,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AR148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AB1" workbookViewId="0">
-      <selection activeCell="AR5" sqref="AR5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18365,7 +18365,7 @@
         <v>5</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>6</v>
@@ -18464,7 +18464,7 @@
         <v>33</v>
       </c>
       <c r="AR1" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:44" x14ac:dyDescent="0.3">

</xml_diff>